<commit_message>
restructure response messages for excel import
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/test_duplicateemail.xlsx
+++ b/src/test/resources/testdata/test_duplicateemail.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -39,13 +39,16 @@
     <t>MANAGER</t>
   </si>
   <si>
-    <t>testuser</t>
-  </si>
-  <si>
     <t>pass11dasdsad</t>
   </si>
   <si>
     <t>test@example.com</t>
+  </si>
+  <si>
+    <t>rownumber</t>
+  </si>
+  <si>
+    <t>testuser3</t>
   </si>
 </sst>
 </file>
@@ -383,55 +386,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
     <col min="2" max="2" width="24.88671875" customWidth="1"/>
     <col min="3" max="3" width="42.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>